<commit_message>
Make graphs to show the difference in number of iterations required to find target between binary chop and linear search
</commit_message>
<xml_diff>
--- a/SearchAndSortingAlgorithms/BinaryChopEfficiencyAnalysis.xlsx
+++ b/SearchAndSortingAlgorithms/BinaryChopEfficiencyAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\C++ Projects -Personal\SearchAndSortingAlgorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BDADB9-AEA2-40CE-B9EE-25561AFFD8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED6687C-FA0A-4FE5-BE24-62613C8420E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5521DD2A-A2D2-433E-BF0D-49967CACE186}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{5521DD2A-A2D2-433E-BF0D-49967CACE186}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="6">
   <si>
     <t>Method</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Number of Iterations</t>
+  </si>
+  <si>
+    <t>Average Iterations to find target</t>
   </si>
 </sst>
 </file>
@@ -104,6 +107,2873 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Linear</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Search</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$75:$B$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68000</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71000</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73000</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74000</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$75:$C$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1601</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2601</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3401</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3601</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4201</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4401</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4601</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4801</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5201</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5401</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5601</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5801</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6201</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6401</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6601</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6801</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7201</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7401</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7601</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7801</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8201</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8401</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8601</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8801</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9201</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9401</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9601</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9801</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10201</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10401</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10601</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10801</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>11001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11201</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11401</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11601</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11801</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>12001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>12201</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12401</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>12601</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>12801</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>13001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>13201</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>13401</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>13601</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>13801</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>14001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>14201</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>14401</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>14601</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>14801</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>15001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D58F-4FC5-A112-4FFA3BCF286A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="lt1">
+                      <a:alpha val="0"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="1235931151"/>
+        <c:axId val="1235931631"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1235931151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Target</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1235931631"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1235931631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1235931151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68000</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71000</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-96F4-40D1-A440-2DCA8188C606}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1407717375"/>
+        <c:axId val="1407718815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1407717375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Target</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1407718815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1407718815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1407717375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="229">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5DBD136-DFF8-FE1E-D36F-3B7760A2D362}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C01399-EF96-D379-4CD0-483BA0D29CB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,30 +3293,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E435821C-5511-499A-99A4-05A9ACE0E357}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -456,8 +3333,14 @@
       <c r="C2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -467,8 +3350,16 @@
       <c r="C3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>ROUND(AVERAGE(C3:C74), 2)</f>
+        <v>15.29</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(C75:C149)</f>
+        <v>7601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -479,7 +3370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -490,7 +3381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -501,7 +3392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -512,7 +3403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -523,7 +3414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -534,7 +3425,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -545,7 +3436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -556,7 +3447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -567,7 +3458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -578,7 +3469,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -589,7 +3480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -600,7 +3491,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2075,7 +4966,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>